<commit_message>
Filter out low-value transactions and update fee records
Added a filter in KOTAK_DB.ipynb to exclude transactions with ReceivedAmount less than 400. Updated fee records for student KOLASANI JAHNAVI and removed/added relevant entries in daywise_fees_collection CSVs. Refreshed output reports and Power BI dashboard to reflect these changes.
</commit_message>
<xml_diff>
--- a/output_data/atom_report.xlsx
+++ b/output_data/atom_report.xlsx
@@ -22462,6 +22462,1122 @@
         </is>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>11000316561861</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>1763044851</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>11250.00</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>13-Nov-2025 20:24:29</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Multi</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>108566739973</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>IFSC0000000</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>JAHNAVI KOLASANI</t>
+        </is>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z61" t="inlineStr">
+        <is>
+          <t>9347559040</t>
+        </is>
+      </c>
+      <c r="AA61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI61" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ61" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT61" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA61" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BC61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD61" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE61" t="inlineStr">
+        <is>
+          <t>19295</t>
+        </is>
+      </c>
+      <c r="BF61" t="inlineStr">
+        <is>
+          <t>263081,264584</t>
+        </is>
+      </c>
+      <c r="BG61" t="inlineStr">
+        <is>
+          <t>2037,2044</t>
+        </is>
+      </c>
+      <c r="BH61" t="inlineStr">
+        <is>
+          <t>eleven thousand two hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI61" t="inlineStr">
+        <is>
+          <t>15599</t>
+        </is>
+      </c>
+      <c r="BJ61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS61" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU61" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>11000316561861</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>1763044851</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>10750.00</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>13-Nov-2025 20:24:29</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>VlllX</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>108566739973</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>0899053000000003</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>JAHNAVI KOLASANI</t>
+        </is>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z62" t="inlineStr">
+        <is>
+          <t>9347559040</t>
+        </is>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI62" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ62" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT62" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA62" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BC62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD62" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE62" t="inlineStr">
+        <is>
+          <t>19295</t>
+        </is>
+      </c>
+      <c r="BF62" t="inlineStr">
+        <is>
+          <t>263081,264584</t>
+        </is>
+      </c>
+      <c r="BG62" t="inlineStr">
+        <is>
+          <t>2037,2044</t>
+        </is>
+      </c>
+      <c r="BH62" t="inlineStr">
+        <is>
+          <t>eleven thousand two hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI62" t="inlineStr">
+        <is>
+          <t>15599</t>
+        </is>
+      </c>
+      <c r="BJ62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS62" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU62" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>11000316561861</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>1763044851</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>500.00</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>13-Nov-2025 20:24:29</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>108566739973</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>0899053000000002</t>
+        </is>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>JAHNAVI KOLASANI</t>
+        </is>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z63" t="inlineStr">
+        <is>
+          <t>9347559040</t>
+        </is>
+      </c>
+      <c r="AA63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI63" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ63" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT63" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA63" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BC63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD63" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE63" t="inlineStr">
+        <is>
+          <t>19295</t>
+        </is>
+      </c>
+      <c r="BF63" t="inlineStr">
+        <is>
+          <t>263081,264584</t>
+        </is>
+      </c>
+      <c r="BG63" t="inlineStr">
+        <is>
+          <t>2037,2044</t>
+        </is>
+      </c>
+      <c r="BH63" t="inlineStr">
+        <is>
+          <t>eleven thousand two hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI63" t="inlineStr">
+        <is>
+          <t>15599</t>
+        </is>
+      </c>
+      <c r="BJ63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS63" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU63" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>